<commit_message>
adding wgsam and hake
</commit_message>
<xml_diff>
--- a/Sablefish/Data/2019Sablefish.xlsx
+++ b/Sablefish/Data/2019Sablefish.xlsx
@@ -26121,7 +26121,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C11" sqref="C11"/>
+      <selection pane="topRight" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26683,7 +26683,7 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -26730,7 +26730,7 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12">
         <v>1</v>

</xml_diff>